<commit_message>
added changes to test results and added pictures
</commit_message>
<xml_diff>
--- a/Test Results/MIDI_Latency/midi_latency_raw_data.xlsx
+++ b/Test Results/MIDI_Latency/midi_latency_raw_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\houdi\Documents\GitHub\Teensy-Synth-Project\Test Results\MIDI_Latency\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F0B3B79-811B-43E8-B876-0CE8A15D04D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAACDD26-69CD-4208-92A7-D4FE706FAD4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D841F286-DFF9-4B60-82B3-63F6FBEE2E2C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Velocity</t>
   </si>
@@ -44,19 +44,22 @@
     <t>MIDI Note</t>
   </si>
   <si>
-    <t>Measured Latency (ms)</t>
-  </si>
-  <si>
     <t>Comments / Observations</t>
   </si>
   <si>
     <t>Test #</t>
   </si>
   <si>
-    <t>ALL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">around 1 micro second from read to osclator </t>
+    <t>C4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">snaping back and forth between two </t>
+  </si>
+  <si>
+    <t>Measured Latency (micro seconds)</t>
+  </si>
+  <si>
+    <t>C4/D4</t>
   </si>
 </sst>
 </file>
@@ -428,7 +431,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{934E1902-B26F-43A9-BA51-D8879771887D}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
@@ -444,7 +447,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -453,18 +456,41 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>90</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
-        <v>6</v>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>90</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>